<commit_message>
update doc listing table
</commit_message>
<xml_diff>
--- a/docs/docs.xlsx
+++ b/docs/docs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwseitz/git/cwseitz.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAD92BC4-83D2-854B-B4FF-6F39764C968C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CB5151-2CBB-344C-A59F-A128778BA1E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="123">
   <si>
     <t>programming</t>
   </si>
@@ -52,9 +52,6 @@
     <t>deep-learning-backprop</t>
   </si>
   <si>
-    <t>gaussian-beams</t>
-  </si>
-  <si>
     <t>fourier-analysis-of-digital-images</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>c-vs-python-bubble-sort-performance</t>
   </si>
   <si>
-    <t>information-theory-basics</t>
-  </si>
-  <si>
     <t>localization-error</t>
   </si>
   <si>
@@ -85,33 +79,21 @@
     <t>how-to-install-c-kernel-in-jupyter</t>
   </si>
   <si>
-    <t>stochastic-gradient-descent</t>
-  </si>
-  <si>
     <t>introduction-to-fast-fourier-transforms-fft</t>
   </si>
   <si>
-    <t>simulating-a-transformer-in-ltspice</t>
-  </si>
-  <si>
     <t>learning-theory</t>
   </si>
   <si>
     <t>electric-and-magnetic-fields-in-a-dielectric-medium</t>
   </si>
   <si>
-    <t>solving-an-lrc-circuit</t>
-  </si>
-  <si>
     <t>fundamentals-of-deep-learning</t>
   </si>
   <si>
     <t>characterizing-digital-ccdcmos-light-sensors</t>
   </si>
   <si>
-    <t>recurrent-neural-networks</t>
-  </si>
-  <si>
     <t>brownian-motion-the-langevin-equation</t>
   </si>
   <si>
@@ -229,23 +211,191 @@
     <t>title</t>
   </si>
   <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Clayton Seitz</t>
-  </si>
-  <si>
-    <t>David McAllester</t>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>The Python/C API</t>
+  </si>
+  <si>
+    <t>TCP/IP Networking Programming</t>
+  </si>
+  <si>
+    <t>Introduction to C</t>
+  </si>
+  <si>
+    <t>C/Python Bubble Sort</t>
+  </si>
+  <si>
+    <t>C Kernel in Jupyter</t>
+  </si>
+  <si>
+    <t>Attention is all you need</t>
+  </si>
+  <si>
+    <t>Backpropagation</t>
+  </si>
+  <si>
+    <t>Regularization</t>
+  </si>
+  <si>
+    <t>Learning Theory</t>
+  </si>
+  <si>
+    <t>Deep Learning Fundamentals</t>
+  </si>
+  <si>
+    <t>Actor-Critic Algorithms</t>
+  </si>
+  <si>
+    <t>Alpha-Beta Algorithm</t>
+  </si>
+  <si>
+    <t>Alpha-Go</t>
+  </si>
+  <si>
+    <t>Alpha-Star</t>
+  </si>
+  <si>
+    <t>Backpropagation 2</t>
+  </si>
+  <si>
+    <t>solving-an-lrc-circuits</t>
+  </si>
+  <si>
+    <t>Convolutional Neural Networks</t>
+  </si>
+  <si>
+    <t>Convolutional Neural Networks 2</t>
+  </si>
+  <si>
+    <t>Mode Collapse</t>
+  </si>
+  <si>
+    <t>Contrasive GANs</t>
+  </si>
+  <si>
+    <t>CTC</t>
+  </si>
+  <si>
+    <t>Graphical Algorithms</t>
+  </si>
+  <si>
+    <t>Graphical Algorithms 2</t>
+  </si>
+  <si>
+    <t>Graphical Algorithms 3</t>
+  </si>
+  <si>
+    <t>Double Descent</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t>Early Stopping</t>
+  </si>
+  <si>
+    <t>Early Stopping 2</t>
+  </si>
+  <si>
+    <t>EDF Framework</t>
+  </si>
+  <si>
+    <t>Einstein Notation</t>
+  </si>
+  <si>
+    <t>Evidence Lower Bound</t>
+  </si>
+  <si>
+    <t>Gradient Flow</t>
+  </si>
+  <si>
+    <t>Deep Learning Frameworks</t>
+  </si>
+  <si>
+    <t>Deep Learning Fundamentals 2</t>
+  </si>
+  <si>
+    <t>GANs</t>
+  </si>
+  <si>
+    <t>GANs 2</t>
+  </si>
+  <si>
+    <t>Gaussian RDAs</t>
+  </si>
+  <si>
+    <t>Thermodynamics in Deep Learning</t>
+  </si>
+  <si>
+    <t>Highway</t>
+  </si>
+  <si>
+    <t>History of Deep Learning</t>
+  </si>
+  <si>
+    <t>Implicit Regularization</t>
+  </si>
+  <si>
+    <t>Optical Instrumentation</t>
+  </si>
+  <si>
+    <t>Mean Squared Displacement</t>
+  </si>
+  <si>
+    <t>Localization Errror</t>
+  </si>
+  <si>
+    <t>1D Fast Fourier Transforms (FFT)</t>
+  </si>
+  <si>
+    <t>EM-Fields in a Dielectric</t>
+  </si>
+  <si>
+    <t>Light Sensors</t>
+  </si>
+  <si>
+    <t>The Langevin Equation</t>
+  </si>
+  <si>
+    <t>Electrodynamics in Isotropic Media</t>
+  </si>
+  <si>
+    <t>Photon Statistics</t>
+  </si>
+  <si>
+    <t>Neuroelectronics</t>
+  </si>
+  <si>
+    <t>2D Fast Fourier Transforms (FFT)</t>
+  </si>
+  <si>
+    <t>RC Frequency Response</t>
+  </si>
+  <si>
+    <t>Analog Impulse Response</t>
+  </si>
+  <si>
+    <t>LRC Circuits</t>
+  </si>
+  <si>
+    <t>Circuits</t>
+  </si>
+  <si>
+    <t>Classical</t>
+  </si>
+  <si>
+    <t>Decoupling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -376,6 +526,18 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -722,9 +884,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1079,36 +1242,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="3" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" width="44.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1119,7 +1283,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1127,10 +1291,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1138,10 +1302,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -1149,10 +1313,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1163,7 +1327,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -1182,10 +1346,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -1193,10 +1357,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1204,10 +1368,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1215,10 +1379,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1229,7 +1393,7 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1240,7 +1404,7 @@
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1248,10 +1412,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -1259,10 +1423,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -1270,10 +1434,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -1281,10 +1445,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -1292,10 +1456,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1303,10 +1467,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1314,10 +1478,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1325,10 +1489,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1336,10 +1500,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1347,10 +1511,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -1358,10 +1522,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -1369,10 +1533,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -1380,10 +1544,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -1391,10 +1555,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -1402,10 +1566,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -1413,10 +1577,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -1424,10 +1588,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -1435,10 +1599,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -1446,10 +1610,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -1457,10 +1621,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -1468,10 +1632,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -1479,10 +1643,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -1490,10 +1654,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -1501,10 +1665,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -1512,10 +1676,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
@@ -1523,10 +1687,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -1534,10 +1698,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
@@ -1545,10 +1709,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -1556,10 +1720,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -1567,10 +1731,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
@@ -1578,10 +1742,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
@@ -1589,10 +1753,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
@@ -1600,43 +1764,43 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -1644,10 +1808,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -1655,10 +1819,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
@@ -1666,10 +1830,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
@@ -1677,10 +1841,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
@@ -1688,10 +1852,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
@@ -1699,115 +1863,61 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="B60" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>15</v>
-      </c>
-      <c r="B62" t="s">
-        <v>71</v>
-      </c>
-      <c r="C62" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>23</v>
-      </c>
-      <c r="B64" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add nat image stats book
</commit_message>
<xml_diff>
--- a/docs/docs.xlsx
+++ b/docs/docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwseitz/git/cwseitz.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3951C28D-5824-3041-B73C-2D85C859E0F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650C6229-6557-0447-8877-5E9727AA9970}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="128">
   <si>
     <t>programming</t>
   </si>
@@ -398,6 +398,12 @@
   </si>
   <si>
     <t>neuroscience</t>
+  </si>
+  <si>
+    <t>natural-image-statistics</t>
+  </si>
+  <si>
+    <t>Natural Image Statistics</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1936,6 +1942,17 @@
         <v>125</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update doc listing page
</commit_message>
<xml_diff>
--- a/docs/docs.xlsx
+++ b/docs/docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwseitz/git/cwseitz.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650C6229-6557-0447-8877-5E9727AA9970}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7EE38F-8432-B443-9083-275A5BF52237}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2720" yWindow="760" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="134">
   <si>
     <t>programming</t>
   </si>
@@ -404,6 +404,24 @@
   </si>
   <si>
     <t>Natural Image Statistics</t>
+  </si>
+  <si>
+    <t>information-theory-elements</t>
+  </si>
+  <si>
+    <t>Elements of Information Theory</t>
+  </si>
+  <si>
+    <t>information-theory</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>NURB 31800</t>
   </si>
 </sst>
 </file>
@@ -1258,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,9 +1287,10 @@
     <col min="1" max="1" width="44.83203125" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -1281,8 +1300,11 @@
       <c r="C1" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1292,8 +1314,11 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1303,8 +1328,11 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1314,8 +1342,11 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1325,8 +1356,11 @@
       <c r="C5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1336,8 +1370,11 @@
       <c r="C6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1347,8 +1384,11 @@
       <c r="C7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1358,8 +1398,11 @@
       <c r="C8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1369,8 +1412,11 @@
       <c r="C9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1380,8 +1426,11 @@
       <c r="C10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1391,8 +1440,11 @@
       <c r="C11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1402,8 +1454,11 @@
       <c r="C12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1413,8 +1468,11 @@
       <c r="C13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1424,8 +1482,11 @@
       <c r="C14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1435,8 +1496,11 @@
       <c r="C15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1446,8 +1510,11 @@
       <c r="C16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1457,8 +1524,11 @@
       <c r="C17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1468,8 +1538,11 @@
       <c r="C18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1479,8 +1552,11 @@
       <c r="C19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1490,8 +1566,11 @@
       <c r="C20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1501,8 +1580,11 @@
       <c r="C21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1512,8 +1594,11 @@
       <c r="C22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1523,8 +1608,11 @@
       <c r="C23" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1534,8 +1622,11 @@
       <c r="C24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1545,8 +1636,11 @@
       <c r="C25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1556,8 +1650,11 @@
       <c r="C26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1567,8 +1664,11 @@
       <c r="C27" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1578,8 +1678,11 @@
       <c r="C28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1589,8 +1692,11 @@
       <c r="C29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -1600,8 +1706,11 @@
       <c r="C30" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1611,8 +1720,11 @@
       <c r="C31" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1622,8 +1734,11 @@
       <c r="C32" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1633,8 +1748,11 @@
       <c r="C33" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -1644,8 +1762,11 @@
       <c r="C34" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1655,8 +1776,11 @@
       <c r="C35" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -1666,8 +1790,11 @@
       <c r="C36" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1677,8 +1804,11 @@
       <c r="C37" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -1688,8 +1818,11 @@
       <c r="C38" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -1699,8 +1832,11 @@
       <c r="C39" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -1710,8 +1846,11 @@
       <c r="C40" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -1721,8 +1860,11 @@
       <c r="C41" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -1732,8 +1874,11 @@
       <c r="C42" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -1743,8 +1888,11 @@
       <c r="C43" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -1754,8 +1902,11 @@
       <c r="C44" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -1765,8 +1916,11 @@
       <c r="C45" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -1776,8 +1930,11 @@
       <c r="C46" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1787,8 +1944,11 @@
       <c r="C47" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -1798,8 +1958,11 @@
       <c r="C48" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -1809,8 +1972,11 @@
       <c r="C49" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -1820,8 +1986,11 @@
       <c r="C50" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>21</v>
       </c>
@@ -1831,8 +2000,11 @@
       <c r="C51" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -1842,8 +2014,11 @@
       <c r="C52" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -1853,8 +2028,11 @@
       <c r="C53" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -1864,8 +2042,11 @@
       <c r="C54" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -1875,8 +2056,11 @@
       <c r="C55" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1886,8 +2070,11 @@
       <c r="C56" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -1897,8 +2084,11 @@
       <c r="C57" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -1908,8 +2098,11 @@
       <c r="C58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -1919,8 +2112,11 @@
       <c r="C59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>80</v>
       </c>
@@ -1930,8 +2126,11 @@
       <c r="C60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -1941,8 +2140,11 @@
       <c r="C61" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>126</v>
       </c>
@@ -1951,6 +2153,23 @@
       </c>
       <c r="C62" t="s">
         <v>125</v>
+      </c>
+      <c r="D62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add deep learning psets
</commit_message>
<xml_diff>
--- a/docs/docs.xlsx
+++ b/docs/docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwseitz/git/cwseitz.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5790CF7-86A5-B845-B52B-03CAA7A4209D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08077505-3F05-3B4E-B4D0-182AC222D7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="760" windowWidth="33520" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="144">
   <si>
     <t>programming</t>
   </si>
@@ -428,6 +428,30 @@
   </si>
   <si>
     <t>Research</t>
+  </si>
+  <si>
+    <t>dl-ps1</t>
+  </si>
+  <si>
+    <t>dl-ps2</t>
+  </si>
+  <si>
+    <t>dl-ps3</t>
+  </si>
+  <si>
+    <t>dl-ps4</t>
+  </si>
+  <si>
+    <t>Training a MLP</t>
+  </si>
+  <si>
+    <t>Training a CNN</t>
+  </si>
+  <si>
+    <t>Training a GAN/VAE</t>
+  </si>
+  <si>
+    <t>Thermodynamics of SGD</t>
   </si>
 </sst>
 </file>
@@ -1290,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2186,6 +2210,62 @@
         <v>135</v>
       </c>
     </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add einstein phil article
</commit_message>
<xml_diff>
--- a/docs/docs.xlsx
+++ b/docs/docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwseitz/git/cwseitz.github.io/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08077505-3F05-3B4E-B4D0-182AC222D7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2027C240-F123-5C42-81D6-84607FC98743}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="760" windowWidth="33520" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="147">
   <si>
     <t>programming</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>Thermodynamics of SGD</t>
+  </si>
+  <si>
+    <t>What I Believe - Einstein</t>
+  </si>
+  <si>
+    <t>what-i-believe</t>
+  </si>
+  <si>
+    <t>philosophy</t>
   </si>
 </sst>
 </file>
@@ -1314,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2266,6 +2275,20 @@
         <v>134</v>
       </c>
     </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>